<commit_message>
excel bom v1.2 for all pcbs
</commit_message>
<xml_diff>
--- a/parts/lc256_v12_bom_all.xlsx
+++ b/parts/lc256_v12_bom_all.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vossi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vossi/--development/lc256-computer/parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB5794-5A38-BC49-89B7-34850542E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E591CBBA-B67E-3645-9343-99FE7BD64F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23960" yWindow="1260" windowWidth="23100" windowHeight="16700" xr2:uid="{D06CE81A-DE5F-1E43-8D15-8E3E3F081FC9}"/>
   </bookViews>
@@ -1801,9 +1801,6 @@
     <t>3.5mm stereo audio jack black</t>
   </si>
   <si>
-    <t>DS-8-101 270 Deg, Yamaha MSX RGB standard</t>
-  </si>
-  <si>
     <t>DS-6-102, or from C64/1541 board</t>
   </si>
   <si>
@@ -1937,6 +1934,9 @@
   </si>
   <si>
     <t>alternate dual-power LED</t>
+  </si>
+  <si>
+    <t>DS-8-101 270 Deg, Panasonic MSX RGB standard</t>
   </si>
 </sst>
 </file>
@@ -2325,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F4230-F2D2-7841-881B-60FABC8B499C}">
   <dimension ref="A1:E286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4112,7 +4112,7 @@
         <v>219</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -4129,7 +4129,7 @@
         <v>223</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>571</v>
+        <v>616</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
         <v>226</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -4177,7 +4177,7 @@
         <v>234</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -4194,7 +4194,7 @@
         <v>234</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -4211,7 +4211,7 @@
         <v>234</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -4228,7 +4228,7 @@
         <v>234</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -4245,7 +4245,7 @@
         <v>234</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -4262,7 +4262,7 @@
         <v>234</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -4279,7 +4279,7 @@
         <v>234</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -4296,7 +4296,7 @@
         <v>250</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -4381,7 +4381,7 @@
         <v>264</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -4398,7 +4398,7 @@
         <v>266</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -4415,7 +4415,7 @@
         <v>266</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -4432,7 +4432,7 @@
         <v>270</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -4449,7 +4449,7 @@
         <v>266</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -4466,7 +4466,7 @@
         <v>270</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -4483,7 +4483,7 @@
         <v>270</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -4500,7 +4500,7 @@
         <v>270</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -4517,7 +4517,7 @@
         <v>270</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -4534,7 +4534,7 @@
         <v>266</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -4551,7 +4551,7 @@
         <v>270</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -4568,7 +4568,7 @@
         <v>270</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -4585,7 +4585,7 @@
         <v>270</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -4602,7 +4602,7 @@
         <v>270</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -4619,7 +4619,7 @@
         <v>293</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -4636,7 +4636,7 @@
         <v>264</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -4653,7 +4653,7 @@
         <v>264</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -4670,7 +4670,7 @@
         <v>264</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -4687,7 +4687,7 @@
         <v>264</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
         <v>300</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>266</v>
@@ -4704,7 +4704,7 @@
         <v>266</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -4712,7 +4712,7 @@
         <v>301</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>266</v>
@@ -4721,7 +4721,7 @@
         <v>266</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -4738,7 +4738,7 @@
         <v>270</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -4755,7 +4755,7 @@
         <v>266</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -4772,7 +4772,7 @@
         <v>234</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -4789,7 +4789,7 @@
         <v>266</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -4806,7 +4806,7 @@
         <v>266</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -4823,7 +4823,7 @@
         <v>266</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -4831,7 +4831,7 @@
         <v>312</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>270</v>
@@ -4840,7 +4840,7 @@
         <v>270</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -4848,7 +4848,7 @@
         <v>313</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>270</v>
@@ -4857,7 +4857,7 @@
         <v>270</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -4865,7 +4865,7 @@
         <v>314</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>270</v>
@@ -4874,7 +4874,7 @@
         <v>270</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -4882,7 +4882,7 @@
         <v>315</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>270</v>
@@ -4891,7 +4891,7 @@
         <v>270</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -4908,7 +4908,7 @@
         <v>318</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -4925,7 +4925,7 @@
         <v>318</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -4942,7 +4942,7 @@
         <v>318</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -4959,7 +4959,7 @@
         <v>326</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
         <v>326</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -4993,7 +4993,7 @@
         <v>326</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -5010,7 +5010,7 @@
         <v>805</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>431</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -6136,7 +6136,7 @@
         <v>435</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -6153,7 +6153,7 @@
         <v>435</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -6272,7 +6272,7 @@
         <v>453</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
@@ -6283,7 +6283,7 @@
         <v>458</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
@@ -6297,7 +6297,7 @@
         <v>514</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
@@ -6327,13 +6327,13 @@
         <v>455</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>457</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
74AHCT245NS = small version SO20-200mil
</commit_message>
<xml_diff>
--- a/parts/lc256_v12_bom_all.xlsx
+++ b/parts/lc256_v12_bom_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vossi/--development/lc256-computer/parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2465A1-5F58-684C-82DC-20ED437B2B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AF453B-E0C0-FD48-A30D-38D6B21A519E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7560" yWindow="1940" windowWidth="23100" windowHeight="16700" xr2:uid="{D06CE81A-DE5F-1E43-8D15-8E3E3F081FC9}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="618">
   <si>
     <t>Part</t>
   </si>
@@ -1937,6 +1937,9 @@
   </si>
   <si>
     <t>not needed!</t>
+  </si>
+  <si>
+    <t>74AHCT245NS</t>
   </si>
 </sst>
 </file>
@@ -2332,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F4230-F2D2-7841-881B-60FABC8B499C}">
   <dimension ref="A1:E286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3833,7 +3836,7 @@
         <v>168</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>169</v>
+        <v>617</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>169</v>
@@ -3850,7 +3853,7 @@
         <v>171</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>169</v>
+        <v>617</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>169</v>
@@ -3867,7 +3870,7 @@
         <v>172</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>169</v>
+        <v>617</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>169</v>

</xml_diff>